<commit_message>
Fixed Model and data extraction
</commit_message>
<xml_diff>
--- a/data/SmallProb_Data.xlsx
+++ b/data/SmallProb_Data.xlsx
@@ -124,9 +124,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>199440</xdr:colOff>
+      <xdr:colOff>198360</xdr:colOff>
       <xdr:row>21</xdr:row>
-      <xdr:rowOff>142200</xdr:rowOff>
+      <xdr:rowOff>141120</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -139,8 +139,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="612000" y="1714680"/>
-          <a:ext cx="2036160" cy="2428200"/>
+          <a:off x="774000" y="1714680"/>
+          <a:ext cx="2520720" cy="2427120"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -163,10 +163,10 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H11" activeCellId="1" sqref="CV1:CV100 H11"/>
+      <selection pane="topLeft" activeCell="H11" activeCellId="1" sqref="CV:CV H11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.70703125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
@@ -184,13 +184,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:CU100"/>
+  <dimension ref="A1:CV100"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="CF1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="CV100" activeCellId="0" sqref="CV1:CV100"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="CK90" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="CV90" activeCellId="0" sqref="CV:CV"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.70703125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="n">
@@ -490,6 +490,9 @@
       <c r="CU1" s="0" t="n">
         <v>10000</v>
       </c>
+      <c r="CV1" s="0" t="n">
+        <v>10000</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="n">
@@ -789,6 +792,9 @@
       <c r="CU2" s="0" t="n">
         <v>10000</v>
       </c>
+      <c r="CV2" s="0" t="n">
+        <v>10000</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="n">
@@ -1088,6 +1094,9 @@
       <c r="CU3" s="0" t="n">
         <v>10000</v>
       </c>
+      <c r="CV3" s="0" t="n">
+        <v>10000</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="n">
@@ -1387,6 +1396,9 @@
       <c r="CU4" s="0" t="n">
         <v>10000</v>
       </c>
+      <c r="CV4" s="0" t="n">
+        <v>10000</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="n">
@@ -1686,6 +1698,9 @@
       <c r="CU5" s="0" t="n">
         <v>10000</v>
       </c>
+      <c r="CV5" s="0" t="n">
+        <v>10000</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="n">
@@ -1985,6 +2000,9 @@
       <c r="CU6" s="0" t="n">
         <v>10000</v>
       </c>
+      <c r="CV6" s="0" t="n">
+        <v>10000</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="n">
@@ -2284,6 +2302,9 @@
       <c r="CU7" s="0" t="n">
         <v>10000</v>
       </c>
+      <c r="CV7" s="0" t="n">
+        <v>10000</v>
+      </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="n">
@@ -2583,6 +2604,9 @@
       <c r="CU8" s="0" t="n">
         <v>10000</v>
       </c>
+      <c r="CV8" s="0" t="n">
+        <v>10000</v>
+      </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="n">
@@ -2882,6 +2906,9 @@
       <c r="CU9" s="0" t="n">
         <v>10000</v>
       </c>
+      <c r="CV9" s="0" t="n">
+        <v>10000</v>
+      </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="n">
@@ -3181,6 +3208,9 @@
       <c r="CU10" s="0" t="n">
         <v>10000</v>
       </c>
+      <c r="CV10" s="0" t="n">
+        <v>10000</v>
+      </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="n">
@@ -3480,6 +3510,9 @@
       <c r="CU11" s="0" t="n">
         <v>10000</v>
       </c>
+      <c r="CV11" s="0" t="n">
+        <v>10000</v>
+      </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="n">
@@ -3779,6 +3812,9 @@
       <c r="CU12" s="0" t="n">
         <v>10000</v>
       </c>
+      <c r="CV12" s="0" t="n">
+        <v>10000</v>
+      </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="n">
@@ -4078,6 +4114,9 @@
       <c r="CU13" s="0" t="n">
         <v>10000</v>
       </c>
+      <c r="CV13" s="0" t="n">
+        <v>10000</v>
+      </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="n">
@@ -4377,6 +4416,9 @@
       <c r="CU14" s="0" t="n">
         <v>10000</v>
       </c>
+      <c r="CV14" s="0" t="n">
+        <v>10000</v>
+      </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="n">
@@ -4676,6 +4718,9 @@
       <c r="CU15" s="0" t="n">
         <v>10000</v>
       </c>
+      <c r="CV15" s="0" t="n">
+        <v>10000</v>
+      </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="n">
@@ -4975,6 +5020,9 @@
       <c r="CU16" s="0" t="n">
         <v>10000</v>
       </c>
+      <c r="CV16" s="0" t="n">
+        <v>10000</v>
+      </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="n">
@@ -5274,6 +5322,9 @@
       <c r="CU17" s="0" t="n">
         <v>10000</v>
       </c>
+      <c r="CV17" s="0" t="n">
+        <v>10000</v>
+      </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="n">
@@ -5573,6 +5624,9 @@
       <c r="CU18" s="0" t="n">
         <v>10000</v>
       </c>
+      <c r="CV18" s="0" t="n">
+        <v>10000</v>
+      </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="n">
@@ -5872,6 +5926,9 @@
       <c r="CU19" s="0" t="n">
         <v>10000</v>
       </c>
+      <c r="CV19" s="0" t="n">
+        <v>10000</v>
+      </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="n">
@@ -6171,6 +6228,9 @@
       <c r="CU20" s="0" t="n">
         <v>10000</v>
       </c>
+      <c r="CV20" s="0" t="n">
+        <v>10000</v>
+      </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="n">
@@ -6470,6 +6530,9 @@
       <c r="CU21" s="0" t="n">
         <v>10000</v>
       </c>
+      <c r="CV21" s="0" t="n">
+        <v>10000</v>
+      </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="n">
@@ -6769,6 +6832,9 @@
       <c r="CU22" s="0" t="n">
         <v>10000</v>
       </c>
+      <c r="CV22" s="0" t="n">
+        <v>10000</v>
+      </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="n">
@@ -7068,6 +7134,9 @@
       <c r="CU23" s="0" t="n">
         <v>10000</v>
       </c>
+      <c r="CV23" s="0" t="n">
+        <v>10000</v>
+      </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="n">
@@ -7367,6 +7436,9 @@
       <c r="CU24" s="0" t="n">
         <v>10000</v>
       </c>
+      <c r="CV24" s="0" t="n">
+        <v>10000</v>
+      </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="n">
@@ -7666,6 +7738,9 @@
       <c r="CU25" s="0" t="n">
         <v>10000</v>
       </c>
+      <c r="CV25" s="0" t="n">
+        <v>10000</v>
+      </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="n">
@@ -7965,6 +8040,9 @@
       <c r="CU26" s="0" t="n">
         <v>10000</v>
       </c>
+      <c r="CV26" s="0" t="n">
+        <v>10000</v>
+      </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="n">
@@ -8264,6 +8342,9 @@
       <c r="CU27" s="0" t="n">
         <v>10000</v>
       </c>
+      <c r="CV27" s="0" t="n">
+        <v>10000</v>
+      </c>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="n">
@@ -8563,6 +8644,9 @@
       <c r="CU28" s="0" t="n">
         <v>10000</v>
       </c>
+      <c r="CV28" s="0" t="n">
+        <v>10000</v>
+      </c>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="n">
@@ -8862,6 +8946,9 @@
       <c r="CU29" s="0" t="n">
         <v>10000</v>
       </c>
+      <c r="CV29" s="0" t="n">
+        <v>10000</v>
+      </c>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="n">
@@ -9161,6 +9248,9 @@
       <c r="CU30" s="0" t="n">
         <v>10000</v>
       </c>
+      <c r="CV30" s="0" t="n">
+        <v>10000</v>
+      </c>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="n">
@@ -9460,6 +9550,9 @@
       <c r="CU31" s="0" t="n">
         <v>10000</v>
       </c>
+      <c r="CV31" s="0" t="n">
+        <v>10000</v>
+      </c>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="n">
@@ -9759,6 +9852,9 @@
       <c r="CU32" s="0" t="n">
         <v>10000</v>
       </c>
+      <c r="CV32" s="0" t="n">
+        <v>10000</v>
+      </c>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="n">
@@ -10058,6 +10154,9 @@
       <c r="CU33" s="0" t="n">
         <v>10000</v>
       </c>
+      <c r="CV33" s="0" t="n">
+        <v>10000</v>
+      </c>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="n">
@@ -10357,6 +10456,9 @@
       <c r="CU34" s="0" t="n">
         <v>10000</v>
       </c>
+      <c r="CV34" s="0" t="n">
+        <v>10000</v>
+      </c>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="n">
@@ -10656,6 +10758,9 @@
       <c r="CU35" s="0" t="n">
         <v>10000</v>
       </c>
+      <c r="CV35" s="0" t="n">
+        <v>10000</v>
+      </c>
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="n">
@@ -10955,6 +11060,9 @@
       <c r="CU36" s="0" t="n">
         <v>10000</v>
       </c>
+      <c r="CV36" s="0" t="n">
+        <v>10000</v>
+      </c>
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="n">
@@ -11254,6 +11362,9 @@
       <c r="CU37" s="0" t="n">
         <v>10000</v>
       </c>
+      <c r="CV37" s="0" t="n">
+        <v>10000</v>
+      </c>
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="n">
@@ -11553,6 +11664,9 @@
       <c r="CU38" s="0" t="n">
         <v>10000</v>
       </c>
+      <c r="CV38" s="0" t="n">
+        <v>10000</v>
+      </c>
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="n">
@@ -11852,6 +11966,9 @@
       <c r="CU39" s="0" t="n">
         <v>10000</v>
       </c>
+      <c r="CV39" s="0" t="n">
+        <v>10000</v>
+      </c>
     </row>
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="n">
@@ -12151,6 +12268,9 @@
       <c r="CU40" s="0" t="n">
         <v>10000</v>
       </c>
+      <c r="CV40" s="0" t="n">
+        <v>10000</v>
+      </c>
     </row>
     <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="n">
@@ -12450,6 +12570,9 @@
       <c r="CU41" s="0" t="n">
         <v>10000</v>
       </c>
+      <c r="CV41" s="0" t="n">
+        <v>10000</v>
+      </c>
     </row>
     <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="n">
@@ -12749,6 +12872,9 @@
       <c r="CU42" s="0" t="n">
         <v>10000</v>
       </c>
+      <c r="CV42" s="0" t="n">
+        <v>10000</v>
+      </c>
     </row>
     <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="n">
@@ -13048,6 +13174,9 @@
       <c r="CU43" s="0" t="n">
         <v>10000</v>
       </c>
+      <c r="CV43" s="0" t="n">
+        <v>10000</v>
+      </c>
     </row>
     <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="n">
@@ -13347,6 +13476,9 @@
       <c r="CU44" s="0" t="n">
         <v>10000</v>
       </c>
+      <c r="CV44" s="0" t="n">
+        <v>10000</v>
+      </c>
     </row>
     <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="n">
@@ -13646,6 +13778,9 @@
       <c r="CU45" s="0" t="n">
         <v>10000</v>
       </c>
+      <c r="CV45" s="0" t="n">
+        <v>10000</v>
+      </c>
     </row>
     <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="n">
@@ -13945,6 +14080,9 @@
       <c r="CU46" s="0" t="n">
         <v>10000</v>
       </c>
+      <c r="CV46" s="0" t="n">
+        <v>10000</v>
+      </c>
     </row>
     <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="n">
@@ -14244,6 +14382,9 @@
       <c r="CU47" s="0" t="n">
         <v>10000</v>
       </c>
+      <c r="CV47" s="0" t="n">
+        <v>10000</v>
+      </c>
     </row>
     <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="n">
@@ -14543,6 +14684,9 @@
       <c r="CU48" s="0" t="n">
         <v>10000</v>
       </c>
+      <c r="CV48" s="0" t="n">
+        <v>10000</v>
+      </c>
     </row>
     <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="0" t="n">
@@ -14842,6 +14986,9 @@
       <c r="CU49" s="0" t="n">
         <v>10000</v>
       </c>
+      <c r="CV49" s="0" t="n">
+        <v>10000</v>
+      </c>
     </row>
     <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="0" t="n">
@@ -15141,6 +15288,9 @@
       <c r="CU50" s="0" t="n">
         <v>10000</v>
       </c>
+      <c r="CV50" s="0" t="n">
+        <v>10000</v>
+      </c>
     </row>
     <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="0" t="n">
@@ -15440,6 +15590,9 @@
       <c r="CU51" s="0" t="n">
         <v>10000</v>
       </c>
+      <c r="CV51" s="0" t="n">
+        <v>10000</v>
+      </c>
     </row>
     <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="0" t="n">
@@ -15739,6 +15892,9 @@
       <c r="CU52" s="0" t="n">
         <v>10000</v>
       </c>
+      <c r="CV52" s="0" t="n">
+        <v>10000</v>
+      </c>
     </row>
     <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="0" t="n">
@@ -16038,6 +16194,9 @@
       <c r="CU53" s="0" t="n">
         <v>10000</v>
       </c>
+      <c r="CV53" s="0" t="n">
+        <v>10000</v>
+      </c>
     </row>
     <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="0" t="n">
@@ -16337,6 +16496,9 @@
       <c r="CU54" s="0" t="n">
         <v>10000</v>
       </c>
+      <c r="CV54" s="0" t="n">
+        <v>10000</v>
+      </c>
     </row>
     <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="0" t="n">
@@ -16636,6 +16798,9 @@
       <c r="CU55" s="0" t="n">
         <v>10000</v>
       </c>
+      <c r="CV55" s="0" t="n">
+        <v>10000</v>
+      </c>
     </row>
     <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="0" t="n">
@@ -16935,6 +17100,9 @@
       <c r="CU56" s="0" t="n">
         <v>10000</v>
       </c>
+      <c r="CV56" s="0" t="n">
+        <v>10000</v>
+      </c>
     </row>
     <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="0" t="n">
@@ -17234,6 +17402,9 @@
       <c r="CU57" s="0" t="n">
         <v>10000</v>
       </c>
+      <c r="CV57" s="0" t="n">
+        <v>10000</v>
+      </c>
     </row>
     <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="0" t="n">
@@ -17533,6 +17704,9 @@
       <c r="CU58" s="0" t="n">
         <v>10000</v>
       </c>
+      <c r="CV58" s="0" t="n">
+        <v>10000</v>
+      </c>
     </row>
     <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="0" t="n">
@@ -17832,6 +18006,9 @@
       <c r="CU59" s="0" t="n">
         <v>10000</v>
       </c>
+      <c r="CV59" s="0" t="n">
+        <v>10000</v>
+      </c>
     </row>
     <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="0" t="n">
@@ -18131,6 +18308,9 @@
       <c r="CU60" s="0" t="n">
         <v>10000</v>
       </c>
+      <c r="CV60" s="0" t="n">
+        <v>10000</v>
+      </c>
     </row>
     <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="0" t="n">
@@ -18430,6 +18610,9 @@
       <c r="CU61" s="0" t="n">
         <v>10000</v>
       </c>
+      <c r="CV61" s="0" t="n">
+        <v>10000</v>
+      </c>
     </row>
     <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="0" t="n">
@@ -18729,6 +18912,9 @@
       <c r="CU62" s="0" t="n">
         <v>10000</v>
       </c>
+      <c r="CV62" s="0" t="n">
+        <v>10000</v>
+      </c>
     </row>
     <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="0" t="n">
@@ -19028,6 +19214,9 @@
       <c r="CU63" s="0" t="n">
         <v>10000</v>
       </c>
+      <c r="CV63" s="0" t="n">
+        <v>10000</v>
+      </c>
     </row>
     <row r="64" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="0" t="n">
@@ -19327,6 +19516,9 @@
       <c r="CU64" s="0" t="n">
         <v>10000</v>
       </c>
+      <c r="CV64" s="0" t="n">
+        <v>10000</v>
+      </c>
     </row>
     <row r="65" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="0" t="n">
@@ -19626,6 +19818,9 @@
       <c r="CU65" s="0" t="n">
         <v>10000</v>
       </c>
+      <c r="CV65" s="0" t="n">
+        <v>10000</v>
+      </c>
     </row>
     <row r="66" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="0" t="n">
@@ -19925,6 +20120,9 @@
       <c r="CU66" s="0" t="n">
         <v>10000</v>
       </c>
+      <c r="CV66" s="0" t="n">
+        <v>10000</v>
+      </c>
     </row>
     <row r="67" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="0" t="n">
@@ -20224,6 +20422,9 @@
       <c r="CU67" s="0" t="n">
         <v>10000</v>
       </c>
+      <c r="CV67" s="0" t="n">
+        <v>10000</v>
+      </c>
     </row>
     <row r="68" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="0" t="n">
@@ -20523,6 +20724,9 @@
       <c r="CU68" s="0" t="n">
         <v>10000</v>
       </c>
+      <c r="CV68" s="0" t="n">
+        <v>10000</v>
+      </c>
     </row>
     <row r="69" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="0" t="n">
@@ -20822,6 +21026,9 @@
       <c r="CU69" s="0" t="n">
         <v>10000</v>
       </c>
+      <c r="CV69" s="0" t="n">
+        <v>10000</v>
+      </c>
     </row>
     <row r="70" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="0" t="n">
@@ -21121,6 +21328,9 @@
       <c r="CU70" s="0" t="n">
         <v>10000</v>
       </c>
+      <c r="CV70" s="0" t="n">
+        <v>10000</v>
+      </c>
     </row>
     <row r="71" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="0" t="n">
@@ -21420,6 +21630,9 @@
       <c r="CU71" s="0" t="n">
         <v>10000</v>
       </c>
+      <c r="CV71" s="0" t="n">
+        <v>10000</v>
+      </c>
     </row>
     <row r="72" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="0" t="n">
@@ -21719,6 +21932,9 @@
       <c r="CU72" s="0" t="n">
         <v>10000</v>
       </c>
+      <c r="CV72" s="0" t="n">
+        <v>10000</v>
+      </c>
     </row>
     <row r="73" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="0" t="n">
@@ -22018,6 +22234,9 @@
       <c r="CU73" s="0" t="n">
         <v>10000</v>
       </c>
+      <c r="CV73" s="0" t="n">
+        <v>10000</v>
+      </c>
     </row>
     <row r="74" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="0" t="n">
@@ -22317,6 +22536,9 @@
       <c r="CU74" s="0" t="n">
         <v>10000</v>
       </c>
+      <c r="CV74" s="0" t="n">
+        <v>10000</v>
+      </c>
     </row>
     <row r="75" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="0" t="n">
@@ -22616,6 +22838,9 @@
       <c r="CU75" s="0" t="n">
         <v>10000</v>
       </c>
+      <c r="CV75" s="0" t="n">
+        <v>10000</v>
+      </c>
     </row>
     <row r="76" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="0" t="n">
@@ -22915,6 +23140,9 @@
       <c r="CU76" s="0" t="n">
         <v>10000</v>
       </c>
+      <c r="CV76" s="0" t="n">
+        <v>10000</v>
+      </c>
     </row>
     <row r="77" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="0" t="n">
@@ -23214,6 +23442,9 @@
       <c r="CU77" s="0" t="n">
         <v>10000</v>
       </c>
+      <c r="CV77" s="0" t="n">
+        <v>10000</v>
+      </c>
     </row>
     <row r="78" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="0" t="n">
@@ -23513,6 +23744,9 @@
       <c r="CU78" s="0" t="n">
         <v>10000</v>
       </c>
+      <c r="CV78" s="0" t="n">
+        <v>10000</v>
+      </c>
     </row>
     <row r="79" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="0" t="n">
@@ -23812,6 +24046,9 @@
       <c r="CU79" s="0" t="n">
         <v>10000</v>
       </c>
+      <c r="CV79" s="0" t="n">
+        <v>10000</v>
+      </c>
     </row>
     <row r="80" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="0" t="n">
@@ -24111,6 +24348,9 @@
       <c r="CU80" s="0" t="n">
         <v>10000</v>
       </c>
+      <c r="CV80" s="0" t="n">
+        <v>10000</v>
+      </c>
     </row>
     <row r="81" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="0" t="n">
@@ -24410,6 +24650,9 @@
       <c r="CU81" s="0" t="n">
         <v>10000</v>
       </c>
+      <c r="CV81" s="0" t="n">
+        <v>10000</v>
+      </c>
     </row>
     <row r="82" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="0" t="n">
@@ -24709,6 +24952,9 @@
       <c r="CU82" s="0" t="n">
         <v>10000</v>
       </c>
+      <c r="CV82" s="0" t="n">
+        <v>10000</v>
+      </c>
     </row>
     <row r="83" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="0" t="n">
@@ -25008,6 +25254,9 @@
       <c r="CU83" s="0" t="n">
         <v>10000</v>
       </c>
+      <c r="CV83" s="0" t="n">
+        <v>10000</v>
+      </c>
     </row>
     <row r="84" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="0" t="n">
@@ -25307,6 +25556,9 @@
       <c r="CU84" s="0" t="n">
         <v>10000</v>
       </c>
+      <c r="CV84" s="0" t="n">
+        <v>10000</v>
+      </c>
     </row>
     <row r="85" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="0" t="n">
@@ -25606,6 +25858,9 @@
       <c r="CU85" s="0" t="n">
         <v>10000</v>
       </c>
+      <c r="CV85" s="0" t="n">
+        <v>10000</v>
+      </c>
     </row>
     <row r="86" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="0" t="n">
@@ -25905,6 +26160,9 @@
       <c r="CU86" s="0" t="n">
         <v>10000</v>
       </c>
+      <c r="CV86" s="0" t="n">
+        <v>10000</v>
+      </c>
     </row>
     <row r="87" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="0" t="n">
@@ -26204,6 +26462,9 @@
       <c r="CU87" s="0" t="n">
         <v>10000</v>
       </c>
+      <c r="CV87" s="0" t="n">
+        <v>10000</v>
+      </c>
     </row>
     <row r="88" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="0" t="n">
@@ -26503,6 +26764,9 @@
       <c r="CU88" s="0" t="n">
         <v>10000</v>
       </c>
+      <c r="CV88" s="0" t="n">
+        <v>10000</v>
+      </c>
     </row>
     <row r="89" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="0" t="n">
@@ -26802,6 +27066,9 @@
       <c r="CU89" s="0" t="n">
         <v>10000</v>
       </c>
+      <c r="CV89" s="0" t="n">
+        <v>10000</v>
+      </c>
     </row>
     <row r="90" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="0" t="n">
@@ -27101,6 +27368,9 @@
       <c r="CU90" s="0" t="n">
         <v>10000</v>
       </c>
+      <c r="CV90" s="0" t="n">
+        <v>10000</v>
+      </c>
     </row>
     <row r="91" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="0" t="n">
@@ -27400,6 +27670,9 @@
       <c r="CU91" s="0" t="n">
         <v>10000</v>
       </c>
+      <c r="CV91" s="0" t="n">
+        <v>10000</v>
+      </c>
     </row>
     <row r="92" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="0" t="n">
@@ -27699,6 +27972,9 @@
       <c r="CU92" s="0" t="n">
         <v>10000</v>
       </c>
+      <c r="CV92" s="0" t="n">
+        <v>10000</v>
+      </c>
     </row>
     <row r="93" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="0" t="n">
@@ -27998,6 +28274,9 @@
       <c r="CU93" s="0" t="n">
         <v>10000</v>
       </c>
+      <c r="CV93" s="0" t="n">
+        <v>10000</v>
+      </c>
     </row>
     <row r="94" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="0" t="n">
@@ -28297,6 +28576,9 @@
       <c r="CU94" s="0" t="n">
         <v>10000</v>
       </c>
+      <c r="CV94" s="0" t="n">
+        <v>10000</v>
+      </c>
     </row>
     <row r="95" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="0" t="n">
@@ -28596,6 +28878,9 @@
       <c r="CU95" s="0" t="n">
         <v>10000</v>
       </c>
+      <c r="CV95" s="0" t="n">
+        <v>10000</v>
+      </c>
     </row>
     <row r="96" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="0" t="n">
@@ -28895,6 +29180,9 @@
       <c r="CU96" s="0" t="n">
         <v>10000</v>
       </c>
+      <c r="CV96" s="0" t="n">
+        <v>10000</v>
+      </c>
     </row>
     <row r="97" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="0" t="n">
@@ -29194,6 +29482,9 @@
       <c r="CU97" s="0" t="n">
         <v>10000</v>
       </c>
+      <c r="CV97" s="0" t="n">
+        <v>10000</v>
+      </c>
     </row>
     <row r="98" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A98" s="0" t="n">
@@ -29493,6 +29784,9 @@
       <c r="CU98" s="0" t="n">
         <v>10000</v>
       </c>
+      <c r="CV98" s="0" t="n">
+        <v>10000</v>
+      </c>
     </row>
     <row r="99" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A99" s="0" t="n">
@@ -29792,6 +30086,9 @@
       <c r="CU99" s="0" t="n">
         <v>10000</v>
       </c>
+      <c r="CV99" s="0" t="n">
+        <v>10000</v>
+      </c>
     </row>
     <row r="100" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="0" t="n">
@@ -30089,6 +30386,9 @@
         <v>10000</v>
       </c>
       <c r="CU100" s="0" t="n">
+        <v>10000</v>
+      </c>
+      <c r="CV100" s="0" t="n">
         <v>10000</v>
       </c>
     </row>
@@ -30108,13 +30408,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:CU100"/>
+  <dimension ref="A1:CV100"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="CH1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="CV100" activeCellId="0" sqref="CV1:CV100"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="CJ1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="CV1" activeCellId="0" sqref="CV:CV"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.70703125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="n">
@@ -30414,6 +30714,9 @@
       <c r="CU1" s="0" t="n">
         <v>10000</v>
       </c>
+      <c r="CV1" s="0" t="n">
+        <v>10000</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="n">
@@ -30713,6 +31016,9 @@
       <c r="CU2" s="0" t="n">
         <v>10000</v>
       </c>
+      <c r="CV2" s="0" t="n">
+        <v>10000</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="n">
@@ -31012,6 +31318,9 @@
       <c r="CU3" s="0" t="n">
         <v>10000</v>
       </c>
+      <c r="CV3" s="0" t="n">
+        <v>10000</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="n">
@@ -31311,6 +31620,9 @@
       <c r="CU4" s="0" t="n">
         <v>10000</v>
       </c>
+      <c r="CV4" s="0" t="n">
+        <v>10000</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="n">
@@ -31610,6 +31922,9 @@
       <c r="CU5" s="0" t="n">
         <v>10000</v>
       </c>
+      <c r="CV5" s="0" t="n">
+        <v>10000</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="n">
@@ -31909,6 +32224,9 @@
       <c r="CU6" s="0" t="n">
         <v>10000</v>
       </c>
+      <c r="CV6" s="0" t="n">
+        <v>10000</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="n">
@@ -32208,6 +32526,9 @@
       <c r="CU7" s="0" t="n">
         <v>10000</v>
       </c>
+      <c r="CV7" s="0" t="n">
+        <v>10000</v>
+      </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="n">
@@ -32507,6 +32828,9 @@
       <c r="CU8" s="0" t="n">
         <v>10000</v>
       </c>
+      <c r="CV8" s="0" t="n">
+        <v>10000</v>
+      </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="n">
@@ -32806,6 +33130,9 @@
       <c r="CU9" s="0" t="n">
         <v>10000</v>
       </c>
+      <c r="CV9" s="0" t="n">
+        <v>10000</v>
+      </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="n">
@@ -33105,6 +33432,9 @@
       <c r="CU10" s="0" t="n">
         <v>10000</v>
       </c>
+      <c r="CV10" s="0" t="n">
+        <v>10000</v>
+      </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="n">
@@ -33404,6 +33734,9 @@
       <c r="CU11" s="0" t="n">
         <v>10000</v>
       </c>
+      <c r="CV11" s="0" t="n">
+        <v>10000</v>
+      </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="n">
@@ -33703,6 +34036,9 @@
       <c r="CU12" s="0" t="n">
         <v>10000</v>
       </c>
+      <c r="CV12" s="0" t="n">
+        <v>10000</v>
+      </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="n">
@@ -34002,6 +34338,9 @@
       <c r="CU13" s="0" t="n">
         <v>10000</v>
       </c>
+      <c r="CV13" s="0" t="n">
+        <v>10000</v>
+      </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="n">
@@ -34301,6 +34640,9 @@
       <c r="CU14" s="0" t="n">
         <v>10000</v>
       </c>
+      <c r="CV14" s="0" t="n">
+        <v>10000</v>
+      </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="n">
@@ -34600,6 +34942,9 @@
       <c r="CU15" s="0" t="n">
         <v>10000</v>
       </c>
+      <c r="CV15" s="0" t="n">
+        <v>10000</v>
+      </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="n">
@@ -34899,6 +35244,9 @@
       <c r="CU16" s="0" t="n">
         <v>10000</v>
       </c>
+      <c r="CV16" s="0" t="n">
+        <v>10000</v>
+      </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="n">
@@ -35198,6 +35546,9 @@
       <c r="CU17" s="0" t="n">
         <v>10000</v>
       </c>
+      <c r="CV17" s="0" t="n">
+        <v>10000</v>
+      </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="n">
@@ -35497,6 +35848,9 @@
       <c r="CU18" s="0" t="n">
         <v>10000</v>
       </c>
+      <c r="CV18" s="0" t="n">
+        <v>10000</v>
+      </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="n">
@@ -35796,6 +36150,9 @@
       <c r="CU19" s="0" t="n">
         <v>10000</v>
       </c>
+      <c r="CV19" s="0" t="n">
+        <v>10000</v>
+      </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="n">
@@ -36095,6 +36452,9 @@
       <c r="CU20" s="0" t="n">
         <v>10000</v>
       </c>
+      <c r="CV20" s="0" t="n">
+        <v>10000</v>
+      </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="n">
@@ -36394,6 +36754,9 @@
       <c r="CU21" s="0" t="n">
         <v>10000</v>
       </c>
+      <c r="CV21" s="0" t="n">
+        <v>10000</v>
+      </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="n">
@@ -36693,6 +37056,9 @@
       <c r="CU22" s="0" t="n">
         <v>10000</v>
       </c>
+      <c r="CV22" s="0" t="n">
+        <v>10000</v>
+      </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="n">
@@ -36992,6 +37358,9 @@
       <c r="CU23" s="0" t="n">
         <v>10000</v>
       </c>
+      <c r="CV23" s="0" t="n">
+        <v>10000</v>
+      </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="n">
@@ -37291,6 +37660,9 @@
       <c r="CU24" s="0" t="n">
         <v>10000</v>
       </c>
+      <c r="CV24" s="0" t="n">
+        <v>10000</v>
+      </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="n">
@@ -37590,6 +37962,9 @@
       <c r="CU25" s="0" t="n">
         <v>10000</v>
       </c>
+      <c r="CV25" s="0" t="n">
+        <v>10000</v>
+      </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="n">
@@ -37889,6 +38264,9 @@
       <c r="CU26" s="0" t="n">
         <v>10000</v>
       </c>
+      <c r="CV26" s="0" t="n">
+        <v>10000</v>
+      </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="n">
@@ -38188,6 +38566,9 @@
       <c r="CU27" s="0" t="n">
         <v>10000</v>
       </c>
+      <c r="CV27" s="0" t="n">
+        <v>10000</v>
+      </c>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="n">
@@ -38487,6 +38868,9 @@
       <c r="CU28" s="0" t="n">
         <v>10000</v>
       </c>
+      <c r="CV28" s="0" t="n">
+        <v>10000</v>
+      </c>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="n">
@@ -38786,6 +39170,9 @@
       <c r="CU29" s="0" t="n">
         <v>10000</v>
       </c>
+      <c r="CV29" s="0" t="n">
+        <v>10000</v>
+      </c>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="n">
@@ -39085,6 +39472,9 @@
       <c r="CU30" s="0" t="n">
         <v>10000</v>
       </c>
+      <c r="CV30" s="0" t="n">
+        <v>10000</v>
+      </c>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="n">
@@ -39384,6 +39774,9 @@
       <c r="CU31" s="0" t="n">
         <v>10000</v>
       </c>
+      <c r="CV31" s="0" t="n">
+        <v>10000</v>
+      </c>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="n">
@@ -39683,6 +40076,9 @@
       <c r="CU32" s="0" t="n">
         <v>10000</v>
       </c>
+      <c r="CV32" s="0" t="n">
+        <v>10000</v>
+      </c>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="n">
@@ -39982,6 +40378,9 @@
       <c r="CU33" s="0" t="n">
         <v>10000</v>
       </c>
+      <c r="CV33" s="0" t="n">
+        <v>10000</v>
+      </c>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="n">
@@ -40281,6 +40680,9 @@
       <c r="CU34" s="0" t="n">
         <v>10000</v>
       </c>
+      <c r="CV34" s="0" t="n">
+        <v>10000</v>
+      </c>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="n">
@@ -40580,6 +40982,9 @@
       <c r="CU35" s="0" t="n">
         <v>10000</v>
       </c>
+      <c r="CV35" s="0" t="n">
+        <v>10000</v>
+      </c>
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="n">
@@ -40879,6 +41284,9 @@
       <c r="CU36" s="0" t="n">
         <v>10000</v>
       </c>
+      <c r="CV36" s="0" t="n">
+        <v>10000</v>
+      </c>
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="n">
@@ -41178,6 +41586,9 @@
       <c r="CU37" s="0" t="n">
         <v>10000</v>
       </c>
+      <c r="CV37" s="0" t="n">
+        <v>10000</v>
+      </c>
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="n">
@@ -41477,6 +41888,9 @@
       <c r="CU38" s="0" t="n">
         <v>10000</v>
       </c>
+      <c r="CV38" s="0" t="n">
+        <v>10000</v>
+      </c>
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="n">
@@ -41776,6 +42190,9 @@
       <c r="CU39" s="0" t="n">
         <v>10000</v>
       </c>
+      <c r="CV39" s="0" t="n">
+        <v>10000</v>
+      </c>
     </row>
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="n">
@@ -42075,6 +42492,9 @@
       <c r="CU40" s="0" t="n">
         <v>10000</v>
       </c>
+      <c r="CV40" s="0" t="n">
+        <v>10000</v>
+      </c>
     </row>
     <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="n">
@@ -42374,6 +42794,9 @@
       <c r="CU41" s="0" t="n">
         <v>10000</v>
       </c>
+      <c r="CV41" s="0" t="n">
+        <v>10000</v>
+      </c>
     </row>
     <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="n">
@@ -42673,6 +43096,9 @@
       <c r="CU42" s="0" t="n">
         <v>10000</v>
       </c>
+      <c r="CV42" s="0" t="n">
+        <v>10000</v>
+      </c>
     </row>
     <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="n">
@@ -42972,6 +43398,9 @@
       <c r="CU43" s="0" t="n">
         <v>10000</v>
       </c>
+      <c r="CV43" s="0" t="n">
+        <v>10000</v>
+      </c>
     </row>
     <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="n">
@@ -43271,6 +43700,9 @@
       <c r="CU44" s="0" t="n">
         <v>10000</v>
       </c>
+      <c r="CV44" s="0" t="n">
+        <v>10000</v>
+      </c>
     </row>
     <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="n">
@@ -43570,6 +44002,9 @@
       <c r="CU45" s="0" t="n">
         <v>10000</v>
       </c>
+      <c r="CV45" s="0" t="n">
+        <v>10000</v>
+      </c>
     </row>
     <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="n">
@@ -43869,6 +44304,9 @@
       <c r="CU46" s="0" t="n">
         <v>10000</v>
       </c>
+      <c r="CV46" s="0" t="n">
+        <v>10000</v>
+      </c>
     </row>
     <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="n">
@@ -44168,6 +44606,9 @@
       <c r="CU47" s="0" t="n">
         <v>10000</v>
       </c>
+      <c r="CV47" s="0" t="n">
+        <v>10000</v>
+      </c>
     </row>
     <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="n">
@@ -44467,6 +44908,9 @@
       <c r="CU48" s="0" t="n">
         <v>10000</v>
       </c>
+      <c r="CV48" s="0" t="n">
+        <v>10000</v>
+      </c>
     </row>
     <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="0" t="n">
@@ -44766,6 +45210,9 @@
       <c r="CU49" s="0" t="n">
         <v>10000</v>
       </c>
+      <c r="CV49" s="0" t="n">
+        <v>10000</v>
+      </c>
     </row>
     <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="0" t="n">
@@ -45065,6 +45512,9 @@
       <c r="CU50" s="0" t="n">
         <v>10000</v>
       </c>
+      <c r="CV50" s="0" t="n">
+        <v>10000</v>
+      </c>
     </row>
     <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="0" t="n">
@@ -45364,6 +45814,9 @@
       <c r="CU51" s="0" t="n">
         <v>10000</v>
       </c>
+      <c r="CV51" s="0" t="n">
+        <v>10000</v>
+      </c>
     </row>
     <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="0" t="n">
@@ -45663,6 +46116,9 @@
       <c r="CU52" s="0" t="n">
         <v>10000</v>
       </c>
+      <c r="CV52" s="0" t="n">
+        <v>10000</v>
+      </c>
     </row>
     <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="0" t="n">
@@ -45962,6 +46418,9 @@
       <c r="CU53" s="0" t="n">
         <v>10000</v>
       </c>
+      <c r="CV53" s="0" t="n">
+        <v>10000</v>
+      </c>
     </row>
     <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="0" t="n">
@@ -46261,6 +46720,9 @@
       <c r="CU54" s="0" t="n">
         <v>10000</v>
       </c>
+      <c r="CV54" s="0" t="n">
+        <v>10000</v>
+      </c>
     </row>
     <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="0" t="n">
@@ -46560,6 +47022,9 @@
       <c r="CU55" s="0" t="n">
         <v>10000</v>
       </c>
+      <c r="CV55" s="0" t="n">
+        <v>10000</v>
+      </c>
     </row>
     <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="0" t="n">
@@ -46859,6 +47324,9 @@
       <c r="CU56" s="0" t="n">
         <v>10000</v>
       </c>
+      <c r="CV56" s="0" t="n">
+        <v>10000</v>
+      </c>
     </row>
     <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="0" t="n">
@@ -47158,6 +47626,9 @@
       <c r="CU57" s="0" t="n">
         <v>10000</v>
       </c>
+      <c r="CV57" s="0" t="n">
+        <v>10000</v>
+      </c>
     </row>
     <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="0" t="n">
@@ -47457,6 +47928,9 @@
       <c r="CU58" s="0" t="n">
         <v>10000</v>
       </c>
+      <c r="CV58" s="0" t="n">
+        <v>10000</v>
+      </c>
     </row>
     <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="0" t="n">
@@ -47756,6 +48230,9 @@
       <c r="CU59" s="0" t="n">
         <v>10000</v>
       </c>
+      <c r="CV59" s="0" t="n">
+        <v>10000</v>
+      </c>
     </row>
     <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="0" t="n">
@@ -48055,6 +48532,9 @@
       <c r="CU60" s="0" t="n">
         <v>10000</v>
       </c>
+      <c r="CV60" s="0" t="n">
+        <v>10000</v>
+      </c>
     </row>
     <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="0" t="n">
@@ -48354,6 +48834,9 @@
       <c r="CU61" s="0" t="n">
         <v>10000</v>
       </c>
+      <c r="CV61" s="0" t="n">
+        <v>10000</v>
+      </c>
     </row>
     <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="0" t="n">
@@ -48653,6 +49136,9 @@
       <c r="CU62" s="0" t="n">
         <v>10000</v>
       </c>
+      <c r="CV62" s="0" t="n">
+        <v>10000</v>
+      </c>
     </row>
     <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="0" t="n">
@@ -48952,6 +49438,9 @@
       <c r="CU63" s="0" t="n">
         <v>10000</v>
       </c>
+      <c r="CV63" s="0" t="n">
+        <v>10000</v>
+      </c>
     </row>
     <row r="64" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="0" t="n">
@@ -49251,6 +49740,9 @@
       <c r="CU64" s="0" t="n">
         <v>10000</v>
       </c>
+      <c r="CV64" s="0" t="n">
+        <v>10000</v>
+      </c>
     </row>
     <row r="65" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="0" t="n">
@@ -49550,6 +50042,9 @@
       <c r="CU65" s="0" t="n">
         <v>10000</v>
       </c>
+      <c r="CV65" s="0" t="n">
+        <v>10000</v>
+      </c>
     </row>
     <row r="66" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="0" t="n">
@@ -49849,6 +50344,9 @@
       <c r="CU66" s="0" t="n">
         <v>10000</v>
       </c>
+      <c r="CV66" s="0" t="n">
+        <v>10000</v>
+      </c>
     </row>
     <row r="67" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="0" t="n">
@@ -50148,6 +50646,9 @@
       <c r="CU67" s="0" t="n">
         <v>10000</v>
       </c>
+      <c r="CV67" s="0" t="n">
+        <v>10000</v>
+      </c>
     </row>
     <row r="68" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="0" t="n">
@@ -50447,6 +50948,9 @@
       <c r="CU68" s="0" t="n">
         <v>10000</v>
       </c>
+      <c r="CV68" s="0" t="n">
+        <v>10000</v>
+      </c>
     </row>
     <row r="69" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="0" t="n">
@@ -50746,6 +51250,9 @@
       <c r="CU69" s="0" t="n">
         <v>10000</v>
       </c>
+      <c r="CV69" s="0" t="n">
+        <v>10000</v>
+      </c>
     </row>
     <row r="70" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="0" t="n">
@@ -51045,6 +51552,9 @@
       <c r="CU70" s="0" t="n">
         <v>10000</v>
       </c>
+      <c r="CV70" s="0" t="n">
+        <v>10000</v>
+      </c>
     </row>
     <row r="71" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="0" t="n">
@@ -51344,6 +51854,9 @@
       <c r="CU71" s="0" t="n">
         <v>10000</v>
       </c>
+      <c r="CV71" s="0" t="n">
+        <v>10000</v>
+      </c>
     </row>
     <row r="72" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="0" t="n">
@@ -51643,6 +52156,9 @@
       <c r="CU72" s="0" t="n">
         <v>10000</v>
       </c>
+      <c r="CV72" s="0" t="n">
+        <v>10000</v>
+      </c>
     </row>
     <row r="73" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="0" t="n">
@@ -51942,6 +52458,9 @@
       <c r="CU73" s="0" t="n">
         <v>10000</v>
       </c>
+      <c r="CV73" s="0" t="n">
+        <v>10000</v>
+      </c>
     </row>
     <row r="74" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="0" t="n">
@@ -52241,6 +52760,9 @@
       <c r="CU74" s="0" t="n">
         <v>10000</v>
       </c>
+      <c r="CV74" s="0" t="n">
+        <v>10000</v>
+      </c>
     </row>
     <row r="75" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="0" t="n">
@@ -52540,6 +53062,9 @@
       <c r="CU75" s="0" t="n">
         <v>10000</v>
       </c>
+      <c r="CV75" s="0" t="n">
+        <v>10000</v>
+      </c>
     </row>
     <row r="76" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="0" t="n">
@@ -52839,6 +53364,9 @@
       <c r="CU76" s="0" t="n">
         <v>10000</v>
       </c>
+      <c r="CV76" s="0" t="n">
+        <v>10000</v>
+      </c>
     </row>
     <row r="77" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="0" t="n">
@@ -53138,6 +53666,9 @@
       <c r="CU77" s="0" t="n">
         <v>10000</v>
       </c>
+      <c r="CV77" s="0" t="n">
+        <v>10000</v>
+      </c>
     </row>
     <row r="78" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="0" t="n">
@@ -53437,6 +53968,9 @@
       <c r="CU78" s="0" t="n">
         <v>10000</v>
       </c>
+      <c r="CV78" s="0" t="n">
+        <v>10000</v>
+      </c>
     </row>
     <row r="79" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="0" t="n">
@@ -53736,6 +54270,9 @@
       <c r="CU79" s="0" t="n">
         <v>10000</v>
       </c>
+      <c r="CV79" s="0" t="n">
+        <v>10000</v>
+      </c>
     </row>
     <row r="80" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="0" t="n">
@@ -54035,6 +54572,9 @@
       <c r="CU80" s="0" t="n">
         <v>10000</v>
       </c>
+      <c r="CV80" s="0" t="n">
+        <v>10000</v>
+      </c>
     </row>
     <row r="81" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="0" t="n">
@@ -54334,6 +54874,9 @@
       <c r="CU81" s="0" t="n">
         <v>10000</v>
       </c>
+      <c r="CV81" s="0" t="n">
+        <v>10000</v>
+      </c>
     </row>
     <row r="82" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="0" t="n">
@@ -54633,6 +55176,9 @@
       <c r="CU82" s="0" t="n">
         <v>10000</v>
       </c>
+      <c r="CV82" s="0" t="n">
+        <v>10000</v>
+      </c>
     </row>
     <row r="83" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="0" t="n">
@@ -54932,6 +55478,9 @@
       <c r="CU83" s="0" t="n">
         <v>10000</v>
       </c>
+      <c r="CV83" s="0" t="n">
+        <v>10000</v>
+      </c>
     </row>
     <row r="84" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="0" t="n">
@@ -55231,6 +55780,9 @@
       <c r="CU84" s="0" t="n">
         <v>10000</v>
       </c>
+      <c r="CV84" s="0" t="n">
+        <v>10000</v>
+      </c>
     </row>
     <row r="85" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="0" t="n">
@@ -55530,6 +56082,9 @@
       <c r="CU85" s="0" t="n">
         <v>10000</v>
       </c>
+      <c r="CV85" s="0" t="n">
+        <v>10000</v>
+      </c>
     </row>
     <row r="86" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="0" t="n">
@@ -55829,6 +56384,9 @@
       <c r="CU86" s="0" t="n">
         <v>10000</v>
       </c>
+      <c r="CV86" s="0" t="n">
+        <v>10000</v>
+      </c>
     </row>
     <row r="87" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="0" t="n">
@@ -56128,6 +56686,9 @@
       <c r="CU87" s="0" t="n">
         <v>10000</v>
       </c>
+      <c r="CV87" s="0" t="n">
+        <v>10000</v>
+      </c>
     </row>
     <row r="88" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="0" t="n">
@@ -56427,6 +56988,9 @@
       <c r="CU88" s="0" t="n">
         <v>10000</v>
       </c>
+      <c r="CV88" s="0" t="n">
+        <v>10000</v>
+      </c>
     </row>
     <row r="89" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="0" t="n">
@@ -56726,6 +57290,9 @@
       <c r="CU89" s="0" t="n">
         <v>10000</v>
       </c>
+      <c r="CV89" s="0" t="n">
+        <v>10000</v>
+      </c>
     </row>
     <row r="90" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="0" t="n">
@@ -57025,6 +57592,9 @@
       <c r="CU90" s="0" t="n">
         <v>10000</v>
       </c>
+      <c r="CV90" s="0" t="n">
+        <v>10000</v>
+      </c>
     </row>
     <row r="91" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="0" t="n">
@@ -57324,6 +57894,9 @@
       <c r="CU91" s="0" t="n">
         <v>10000</v>
       </c>
+      <c r="CV91" s="0" t="n">
+        <v>10000</v>
+      </c>
     </row>
     <row r="92" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="0" t="n">
@@ -57623,6 +58196,9 @@
       <c r="CU92" s="0" t="n">
         <v>10000</v>
       </c>
+      <c r="CV92" s="0" t="n">
+        <v>10000</v>
+      </c>
     </row>
     <row r="93" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="0" t="n">
@@ -57922,6 +58498,9 @@
       <c r="CU93" s="0" t="n">
         <v>10000</v>
       </c>
+      <c r="CV93" s="0" t="n">
+        <v>10000</v>
+      </c>
     </row>
     <row r="94" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="0" t="n">
@@ -58221,6 +58800,9 @@
       <c r="CU94" s="0" t="n">
         <v>10000</v>
       </c>
+      <c r="CV94" s="0" t="n">
+        <v>10000</v>
+      </c>
     </row>
     <row r="95" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="0" t="n">
@@ -58520,6 +59102,9 @@
       <c r="CU95" s="0" t="n">
         <v>10000</v>
       </c>
+      <c r="CV95" s="0" t="n">
+        <v>10000</v>
+      </c>
     </row>
     <row r="96" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="0" t="n">
@@ -58819,6 +59404,9 @@
       <c r="CU96" s="0" t="n">
         <v>10000</v>
       </c>
+      <c r="CV96" s="0" t="n">
+        <v>10000</v>
+      </c>
     </row>
     <row r="97" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="0" t="n">
@@ -59118,6 +59706,9 @@
       <c r="CU97" s="0" t="n">
         <v>10000</v>
       </c>
+      <c r="CV97" s="0" t="n">
+        <v>10000</v>
+      </c>
     </row>
     <row r="98" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A98" s="0" t="n">
@@ -59417,6 +60008,9 @@
       <c r="CU98" s="0" t="n">
         <v>10000</v>
       </c>
+      <c r="CV98" s="0" t="n">
+        <v>10000</v>
+      </c>
     </row>
     <row r="99" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A99" s="0" t="n">
@@ -59716,6 +60310,9 @@
       <c r="CU99" s="0" t="n">
         <v>10000</v>
       </c>
+      <c r="CV99" s="0" t="n">
+        <v>10000</v>
+      </c>
     </row>
     <row r="100" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="0" t="n">
@@ -60013,6 +60610,9 @@
         <v>10000</v>
       </c>
       <c r="CU100" s="0" t="n">
+        <v>10000</v>
+      </c>
+      <c r="CV100" s="0" t="n">
         <v>10000</v>
       </c>
     </row>
@@ -60035,14 +60635,14 @@
   <dimension ref="A1:A100"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="CV1:CV100 A1"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="1" sqref="CV:CV A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.70703125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -60559,14 +61159,14 @@
   <dimension ref="A1:A100"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="CV1:CV100 A1"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="1" sqref="CV:CV A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.70703125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="n">
-        <v>5</v>
+        <v>17</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -61083,10 +61683,10 @@
   <dimension ref="A1:P100"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F15" activeCellId="1" sqref="CV1:CV100 F15"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="CV:CV A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.70703125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="n">
@@ -61102,10 +61702,10 @@
         <v>0</v>
       </c>
       <c r="E1" s="0" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F1" s="0" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G1" s="0" t="n">
         <v>0</v>
@@ -66106,15 +66706,15 @@
   </sheetPr>
   <dimension ref="A1:A100"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A91" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L101" activeCellId="1" sqref="CV1:CV100 L101"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="CV:CV A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.70703125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="n">
-        <v>2</v>
+        <v>10000</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -66454,162 +67054,162 @@
     </row>
     <row r="69" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="0" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="0" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="0" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="0" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="0" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="0" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="0" t="n">
-        <v>7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="0" t="n">
-        <v>8</v>
+        <v>0</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="0" t="n">
-        <v>9</v>
+        <v>0</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="0" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="0" t="n">
-        <v>11</v>
+        <v>0</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="0" t="n">
-        <v>12</v>
+        <v>0</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="0" t="n">
-        <v>13</v>
+        <v>0</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="0" t="n">
-        <v>14</v>
+        <v>0</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="0" t="n">
-        <v>15</v>
+        <v>0</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="0" t="n">
-        <v>16</v>
+        <v>0</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="0" t="n">
-        <v>17</v>
+        <v>0</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="0" t="n">
-        <v>18</v>
+        <v>0</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="0" t="n">
-        <v>19</v>
+        <v>0</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="0" t="n">
-        <v>20</v>
+        <v>0</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="0" t="n">
-        <v>21</v>
+        <v>0</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="0" t="n">
-        <v>22</v>
+        <v>0</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="0" t="n">
-        <v>23</v>
+        <v>0</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="0" t="n">
-        <v>24</v>
+        <v>0</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="0" t="n">
-        <v>25</v>
+        <v>0</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="0" t="n">
-        <v>26</v>
+        <v>0</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="0" t="n">
-        <v>27</v>
+        <v>0</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="0" t="n">
-        <v>28</v>
+        <v>0</v>
       </c>
     </row>
     <row r="97" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="0" t="n">
-        <v>29</v>
+        <v>0</v>
       </c>
     </row>
     <row r="98" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A98" s="0" t="n">
-        <v>30</v>
+        <v>0</v>
       </c>
     </row>
     <row r="99" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A99" s="0" t="n">
-        <v>31</v>
+        <v>0</v>
       </c>
     </row>
     <row r="100" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="0" t="n">
-        <v>32</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>